<commit_message>
Fix upload asset, staff, location
</commit_message>
<xml_diff>
--- a/spotit_asset.xlsx
+++ b/spotit_asset.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="9">
   <si>
     <t xml:space="preserve">KERUSI IKEA</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t xml:space="preserve">AIRCOND CARTRIDGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM_002</t>
   </si>
 </sst>
 </file>
@@ -146,10 +149,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:G4"/>
+  <dimension ref="A2:G28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -159,7 +162,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.29"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.05"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -223,6 +226,486 @@
         <v>10.21</v>
       </c>
       <c r="G4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>11.21</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>12.21</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>13.21</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>14.21</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>15.21</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>16.21</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>17.21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>18.21</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>19.21</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>20.21</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>21.21</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>22.21</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>23.21</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>24.21</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>25.21</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>26.21</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>27.21</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>28.21</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>29.21</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>30.21</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>31.21</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>32.21</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>33.21</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>34.21</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>